<commit_message>
Added couple of troubleshooting records
</commit_message>
<xml_diff>
--- a/MS_PowerShell.xlsx
+++ b/MS_PowerShell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\personalNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF10065-C097-4B30-9B01-A66DBD4A5DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19334E3D-61E9-49D0-92E3-B4C1B05943D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmd" sheetId="1" r:id="rId1"/>
@@ -3676,38 +3676,38 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4463,8 +4463,8 @@
   </sheetPr>
   <dimension ref="A1:AA254"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="K180" sqref="K180"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4480,10 +4480,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="73"/>
+      <c r="B1" s="72"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -4774,48 +4774,48 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="73"/>
+      <c r="B22" s="72"/>
       <c r="U22" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="83" t="s">
+      <c r="A24" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="83" t="s">
+      <c r="B24" s="72"/>
+      <c r="C24" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="83" t="s">
+      <c r="D24" s="72"/>
+      <c r="E24" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="83" t="s">
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="73"/>
+      <c r="I24" s="72"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="75" t="s">
         <v>84</v>
       </c>
       <c r="B25" s="68"/>
-      <c r="C25" s="82" t="s">
+      <c r="C25" s="75" t="s">
         <v>85</v>
       </c>
       <c r="D25" s="68"/>
-      <c r="E25" s="82" t="s">
+      <c r="E25" s="75" t="s">
         <v>86</v>
       </c>
       <c r="F25" s="68"/>
       <c r="G25" s="68"/>
-      <c r="H25" s="82" t="s">
+      <c r="H25" s="75" t="s">
         <v>87</v>
       </c>
       <c r="I25" s="68"/>
@@ -4824,18 +4824,18 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="D27" s="77" t="s">
+      <c r="B27" s="72"/>
+      <c r="D27" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="73"/>
-      <c r="K27" s="78" t="s">
+      <c r="E27" s="72"/>
+      <c r="K27" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="L27" s="73"/>
+      <c r="L27" s="72"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
@@ -4887,10 +4887,10 @@
       <c r="Q30" s="12"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="73"/>
+      <c r="B31" s="72"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
@@ -4943,10 +4943,10 @@
       <c r="Q34" s="12"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="73"/>
+      <c r="B35" s="72"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
@@ -5005,7 +5005,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-      <c r="K39" s="74" t="s">
+      <c r="K39" s="80" t="s">
         <v>108</v>
       </c>
       <c r="L39" s="68"/>
@@ -5090,10 +5090,10 @@
       <c r="Q43" s="12"/>
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="78" t="s">
+      <c r="A45" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="73"/>
+      <c r="B45" s="72"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
@@ -5169,7 +5169,7 @@
       <c r="L49" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M49" s="84" t="s">
+      <c r="M49" s="76" t="s">
         <v>122</v>
       </c>
       <c r="N49" s="68"/>
@@ -5324,18 +5324,18 @@
       <c r="AA56" s="11"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="79" t="s">
+      <c r="A57" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="B57" s="73"/>
-      <c r="C57" s="73"/>
-      <c r="D57" s="73"/>
-      <c r="G57" s="85" t="s">
+      <c r="B57" s="72"/>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72"/>
+      <c r="G57" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="H57" s="73"/>
-      <c r="I57" s="73"/>
-      <c r="J57" s="73"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="72"/>
+      <c r="J57" s="72"/>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="U57" s="5"/>
@@ -5483,14 +5483,14 @@
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
-      <c r="L62" s="81" t="s">
+      <c r="L62" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="M62" s="73"/>
-      <c r="N62" s="73"/>
-      <c r="O62" s="73"/>
-      <c r="P62" s="73"/>
-      <c r="Q62" s="73"/>
+      <c r="M62" s="72"/>
+      <c r="N62" s="72"/>
+      <c r="O62" s="72"/>
+      <c r="P62" s="72"/>
+      <c r="Q62" s="72"/>
       <c r="R62" s="10"/>
       <c r="U62" s="5"/>
       <c r="W62" s="11"/>
@@ -6278,10 +6278,10 @@
       <c r="AA96" s="11"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="80" t="s">
+      <c r="A97" s="83" t="s">
         <v>212</v>
       </c>
-      <c r="B97" s="73"/>
+      <c r="B97" s="72"/>
       <c r="L97" s="11"/>
       <c r="M97" s="11"/>
       <c r="N97" s="11"/>
@@ -6691,7 +6691,7 @@
       <c r="G112" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="H112" s="71" t="s">
+      <c r="H112" s="84" t="s">
         <v>251</v>
       </c>
       <c r="I112" s="68"/>
@@ -7496,10 +7496,10 @@
       <c r="AA142" s="11"/>
     </row>
     <row r="143" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="72" t="s">
+      <c r="A143" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="B143" s="73"/>
+      <c r="B143" s="72"/>
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
       <c r="I143" s="11"/>
@@ -7540,7 +7540,7 @@
       <c r="AA144" s="11"/>
     </row>
     <row r="145" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="74" t="s">
+      <c r="A145" s="80" t="s">
         <v>305</v>
       </c>
       <c r="B145" s="68"/>
@@ -7568,7 +7568,7 @@
       <c r="AA145" s="11"/>
     </row>
     <row r="146" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="74" t="s">
+      <c r="A146" s="80" t="s">
         <v>309</v>
       </c>
       <c r="B146" s="68"/>
@@ -7711,7 +7711,7 @@
       <c r="G156" s="11"/>
     </row>
     <row r="157" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="75" t="s">
+      <c r="A157" s="86" t="s">
         <v>331</v>
       </c>
       <c r="B157" s="68"/>
@@ -7768,7 +7768,7 @@
       </c>
     </row>
     <row r="163" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="74" t="s">
+      <c r="A163" s="80" t="s">
         <v>339</v>
       </c>
       <c r="B163" s="68"/>
@@ -7933,7 +7933,7 @@
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
-      <c r="F178" s="76"/>
+      <c r="F178" s="81"/>
       <c r="G178" s="68"/>
       <c r="L178" s="22" t="s">
         <v>359</v>
@@ -8210,16 +8210,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="G57:J57"/>
+    <mergeCell ref="H112:I113"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A157:F158"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="F178:G179"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A97:B97"/>
     <mergeCell ref="L62:Q62"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:G25"/>
@@ -8228,17 +8229,16 @@
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="K39:L39"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="F178:G179"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="H112:I113"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A157:F158"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="G57:J57"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8321,8 +8321,8 @@
   </sheetPr>
   <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More troubleshooting sections and added ancient Linux notes
</commit_message>
<xml_diff>
--- a/MS_PowerShell.xlsx
+++ b/MS_PowerShell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\personalNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19334E3D-61E9-49D0-92E3-B4C1B05943D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F57A5-2D69-490B-BBEF-7F93FBD128F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cmd" sheetId="1" r:id="rId1"/>
@@ -3676,38 +3676,38 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4055,39 +4055,39 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="3"/>
+    <col min="1" max="16384" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -4103,13 +4103,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>546</v>
       </c>
@@ -4119,17 +4119,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -4138,14 +4138,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
@@ -4153,14 +4153,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
@@ -4190,12 +4190,12 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="3"/>
+    <col min="1" max="16384" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="65" t="s">
         <v>21</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="66"/>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
@@ -4219,7 +4219,7 @@
       <c r="H2" s="66"/>
       <c r="I2" s="66"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
@@ -4245,7 +4245,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -4258,7 +4258,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -4271,7 +4271,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="67" t="s">
         <v>26</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="H7" s="68"/>
       <c r="I7" s="68"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="68"/>
       <c r="C8" s="68"/>
@@ -4295,7 +4295,7 @@
       <c r="H8" s="68"/>
       <c r="I8" s="68"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -4306,7 +4306,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="69" t="s">
         <v>27</v>
       </c>
@@ -4319,7 +4319,7 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>28</v>
       </c>
@@ -4332,7 +4332,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>29</v>
       </c>
@@ -4345,7 +4345,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>30</v>
       </c>
@@ -4358,7 +4358,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
@@ -4371,7 +4371,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>32</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>547</v>
       </c>
@@ -4399,7 +4399,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>33</v>
       </c>
@@ -4416,7 +4416,7 @@
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>36</v>
       </c>
@@ -4431,12 +4431,12 @@
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="17" t="s">
         <v>39</v>
       </c>
@@ -4463,27 +4463,27 @@
   </sheetPr>
   <dimension ref="A1:AA254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="K80" sqref="K80"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3"/>
-    <col min="2" max="2" width="14.28515625" style="3" customWidth="1"/>
-    <col min="3" max="13" width="12.5703125" style="3"/>
-    <col min="14" max="14" width="14.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="3"/>
+    <col min="2" max="2" width="14.33203125" style="3" customWidth="1"/>
+    <col min="3" max="13" width="12.5546875" style="3"/>
+    <col min="14" max="14" width="14.88671875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" style="3" customWidth="1"/>
     <col min="16" max="16" width="14" style="3" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="12.5703125" style="3"/>
+    <col min="17" max="17" width="15.109375" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="72"/>
+      <c r="B1" s="73"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -4493,7 +4493,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>41</v>
       </c>
@@ -4513,7 +4513,7 @@
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>550</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>552</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>554</v>
       </c>
@@ -4561,7 +4561,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>47</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>556</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>54</v>
       </c>
@@ -4618,7 +4618,7 @@
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -4634,7 +4634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>58</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>61</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>557</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>558</v>
       </c>
@@ -4696,7 +4696,7 @@
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>559</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>560</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
@@ -4755,7 +4755,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>75</v>
       </c>
@@ -4773,49 +4773,49 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="72"/>
+      <c r="B22" s="73"/>
       <c r="U22" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="74" t="s">
+      <c r="B24" s="73"/>
+      <c r="C24" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="72"/>
-      <c r="E24" s="74" t="s">
+      <c r="D24" s="73"/>
+      <c r="E24" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="74" t="s">
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="72"/>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="75" t="s">
+      <c r="I24" s="73"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="82" t="s">
         <v>84</v>
       </c>
       <c r="B25" s="68"/>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="82" t="s">
         <v>85</v>
       </c>
       <c r="D25" s="68"/>
-      <c r="E25" s="75" t="s">
+      <c r="E25" s="82" t="s">
         <v>86</v>
       </c>
       <c r="F25" s="68"/>
       <c r="G25" s="68"/>
-      <c r="H25" s="75" t="s">
+      <c r="H25" s="82" t="s">
         <v>87</v>
       </c>
       <c r="I25" s="68"/>
@@ -4823,26 +4823,26 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="79" t="s">
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="D27" s="79" t="s">
+      <c r="B27" s="73"/>
+      <c r="D27" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="K27" s="73" t="s">
+      <c r="E27" s="73"/>
+      <c r="K27" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="L27" s="72"/>
+      <c r="L27" s="73"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>561</v>
       </c>
@@ -4861,7 +4861,7 @@
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="5" t="s">
         <v>93</v>
       </c>
@@ -4875,7 +4875,7 @@
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K30" s="13" t="s">
         <v>95</v>
       </c>
@@ -4886,11 +4886,11 @@
       <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="79" t="s">
+    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="72"/>
+      <c r="B31" s="73"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
@@ -4899,7 +4899,7 @@
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>563</v>
       </c>
@@ -4915,7 +4915,7 @@
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>99</v>
       </c>
@@ -4931,7 +4931,7 @@
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K34" s="13" t="s">
         <v>102</v>
       </c>
@@ -4942,11 +4942,11 @@
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="72"/>
+      <c r="B35" s="73"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
@@ -4955,7 +4955,7 @@
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
     </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>564</v>
       </c>
@@ -4971,7 +4971,7 @@
       <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>565</v>
       </c>
@@ -4987,7 +4987,7 @@
       <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
@@ -4996,7 +4996,7 @@
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>566</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-      <c r="K39" s="80" t="s">
+      <c r="K39" s="74" t="s">
         <v>108</v>
       </c>
       <c r="L39" s="68"/>
@@ -5015,7 +5015,7 @@
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>567</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="P40" s="12"/>
       <c r="Q40" s="12"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>568</v>
       </c>
@@ -5051,7 +5051,7 @@
       <c r="P41" s="12"/>
       <c r="Q41" s="12"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>569</v>
       </c>
@@ -5070,7 +5070,7 @@
       <c r="P42" s="12"/>
       <c r="Q42" s="12"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>111</v>
       </c>
@@ -5089,11 +5089,11 @@
       <c r="P43" s="12"/>
       <c r="Q43" s="12"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="73" t="s">
+    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="B45" s="72"/>
+      <c r="B45" s="73"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
@@ -5102,7 +5102,7 @@
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>114</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>570</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -5152,7 +5152,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
         <v>119</v>
       </c>
@@ -5169,7 +5169,7 @@
       <c r="L49" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M49" s="76" t="s">
+      <c r="M49" s="84" t="s">
         <v>122</v>
       </c>
       <c r="N49" s="68"/>
@@ -5185,7 +5185,7 @@
       <c r="Z49" s="11"/>
       <c r="AA49" s="11"/>
     </row>
-    <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
         <v>124</v>
       </c>
@@ -5207,7 +5207,7 @@
       <c r="Z50" s="11"/>
       <c r="AA50" s="11"/>
     </row>
-    <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
         <v>126</v>
       </c>
@@ -5234,7 +5234,7 @@
       <c r="Z51" s="11"/>
       <c r="AA51" s="11"/>
     </row>
-    <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="27"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -5253,7 +5253,7 @@
       <c r="Z52" s="11"/>
       <c r="AA52" s="11"/>
     </row>
-    <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
         <v>129</v>
       </c>
@@ -5276,7 +5276,7 @@
       <c r="Z53" s="11"/>
       <c r="AA53" s="11"/>
     </row>
-    <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
         <v>131</v>
       </c>
@@ -5299,7 +5299,7 @@
       <c r="Z54" s="11"/>
       <c r="AA54" s="11"/>
     </row>
-    <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="Q55" s="10"/>
@@ -5311,7 +5311,7 @@
       <c r="Z55" s="11"/>
       <c r="AA55" s="11"/>
     </row>
-    <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="Q56" s="10"/>
@@ -5323,19 +5323,19 @@
       <c r="Z56" s="11"/>
       <c r="AA56" s="11"/>
     </row>
-    <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="82" t="s">
+    <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="G57" s="77" t="s">
+      <c r="B57" s="73"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
+      <c r="G57" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="H57" s="72"/>
-      <c r="I57" s="72"/>
-      <c r="J57" s="72"/>
+      <c r="H57" s="73"/>
+      <c r="I57" s="73"/>
+      <c r="J57" s="73"/>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="U57" s="5"/>
@@ -5345,7 +5345,7 @@
       <c r="Z57" s="11"/>
       <c r="AA57" s="11"/>
     </row>
-    <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
         <v>135</v>
       </c>
@@ -5377,7 +5377,7 @@
       <c r="Z58" s="11"/>
       <c r="AA58" s="11"/>
     </row>
-    <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="33" t="s">
         <v>138</v>
       </c>
@@ -5409,7 +5409,7 @@
       <c r="Z59" s="11"/>
       <c r="AA59" s="11"/>
     </row>
-    <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="32"/>
       <c r="B60" s="32"/>
       <c r="C60" s="32"/>
@@ -5439,7 +5439,7 @@
       <c r="Z60" s="11"/>
       <c r="AA60" s="11"/>
     </row>
-    <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="22" t="s">
         <v>142</v>
       </c>
@@ -5469,7 +5469,7 @@
       <c r="Z61" s="11"/>
       <c r="AA61" s="11"/>
     </row>
-    <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="33" t="s">
         <v>143</v>
       </c>
@@ -5483,14 +5483,14 @@
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
-      <c r="L62" s="78" t="s">
+      <c r="L62" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="M62" s="72"/>
-      <c r="N62" s="72"/>
-      <c r="O62" s="72"/>
-      <c r="P62" s="72"/>
-      <c r="Q62" s="72"/>
+      <c r="M62" s="73"/>
+      <c r="N62" s="73"/>
+      <c r="O62" s="73"/>
+      <c r="P62" s="73"/>
+      <c r="Q62" s="73"/>
       <c r="R62" s="10"/>
       <c r="U62" s="5"/>
       <c r="W62" s="11"/>
@@ -5499,7 +5499,7 @@
       <c r="Z62" s="11"/>
       <c r="AA62" s="11"/>
     </row>
-    <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="33" t="s">
         <v>145</v>
       </c>
@@ -5533,7 +5533,7 @@
       <c r="Z63" s="11"/>
       <c r="AA63" s="11"/>
     </row>
-    <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="32"/>
       <c r="B64" s="32"/>
       <c r="C64" s="32"/>
@@ -5567,7 +5567,7 @@
       <c r="Z64" s="11"/>
       <c r="AA64" s="11"/>
     </row>
-    <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="32"/>
       <c r="B65" s="36" t="s">
         <v>154</v>
@@ -5601,7 +5601,7 @@
       <c r="Z65" s="11"/>
       <c r="AA65" s="11"/>
     </row>
-    <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="32"/>
       <c r="B66" s="37" t="s">
         <v>159</v>
@@ -5637,7 +5637,7 @@
       <c r="Z66" s="11"/>
       <c r="AA66" s="11"/>
     </row>
-    <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="32"/>
       <c r="B67" s="33" t="s">
         <v>164</v>
@@ -5669,7 +5669,7 @@
       <c r="Z67" s="11"/>
       <c r="AA67" s="11"/>
     </row>
-    <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="32"/>
       <c r="B68" s="33"/>
       <c r="C68" s="32"/>
@@ -5703,7 +5703,7 @@
       <c r="Z68" s="11"/>
       <c r="AA68" s="11"/>
     </row>
-    <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="32"/>
       <c r="B69" s="37" t="s">
         <v>172</v>
@@ -5737,7 +5737,7 @@
       <c r="Z69" s="11"/>
       <c r="AA69" s="11"/>
     </row>
-    <row r="70" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="32"/>
       <c r="B70" s="33" t="s">
         <v>177</v>
@@ -5767,7 +5767,7 @@
       <c r="Z70" s="11"/>
       <c r="AA70" s="11"/>
     </row>
-    <row r="71" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="32"/>
       <c r="B71" s="33"/>
       <c r="C71" s="32"/>
@@ -5797,7 +5797,7 @@
       <c r="Z71" s="11"/>
       <c r="AA71" s="11"/>
     </row>
-    <row r="72" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="32"/>
       <c r="B72" s="37" t="s">
         <v>180</v>
@@ -5831,7 +5831,7 @@
       <c r="Z72" s="11"/>
       <c r="AA72" s="11"/>
     </row>
-    <row r="73" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="32"/>
       <c r="B73" s="33" t="s">
         <v>184</v>
@@ -5861,7 +5861,7 @@
       <c r="Z73" s="11"/>
       <c r="AA73" s="11"/>
     </row>
-    <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="33"/>
       <c r="B74" s="32"/>
       <c r="C74" s="32"/>
@@ -5892,7 +5892,7 @@
       <c r="Z74" s="11"/>
       <c r="AA74" s="11"/>
     </row>
-    <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="37" t="s">
         <v>75</v>
       </c>
@@ -5925,7 +5925,7 @@
       <c r="Z75" s="11"/>
       <c r="AA75" s="11"/>
     </row>
-    <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="37" t="s">
         <v>192</v>
       </c>
@@ -5958,7 +5958,7 @@
       <c r="Z76" s="11"/>
       <c r="AA76" s="11"/>
     </row>
-    <row r="77" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="33"/>
       <c r="B77" s="32"/>
       <c r="C77" s="32"/>
@@ -5985,7 +5985,7 @@
       <c r="Z77" s="11"/>
       <c r="AA77" s="11"/>
     </row>
-    <row r="78" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="G78" s="15"/>
       <c r="H78" s="15"/>
@@ -6008,7 +6008,7 @@
       <c r="Z78" s="11"/>
       <c r="AA78" s="11"/>
     </row>
-    <row r="79" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="G79" s="15"/>
       <c r="H79" s="15"/>
@@ -6031,7 +6031,7 @@
       <c r="Z79" s="11"/>
       <c r="AA79" s="11"/>
     </row>
-    <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L80" s="15"/>
       <c r="M80" s="15" t="s">
         <v>199</v>
@@ -6048,7 +6048,7 @@
       <c r="Z80" s="11"/>
       <c r="AA80" s="11"/>
     </row>
-    <row r="81" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L81" s="15"/>
       <c r="M81" s="15" t="s">
         <v>200</v>
@@ -6065,7 +6065,7 @@
       <c r="Z81" s="11"/>
       <c r="AA81" s="11"/>
     </row>
-    <row r="82" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
       <c r="N82" s="15"/>
@@ -6080,7 +6080,7 @@
       <c r="Z82" s="11"/>
       <c r="AA82" s="11"/>
     </row>
-    <row r="83" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L83" s="8"/>
       <c r="M83" s="9" t="s">
         <v>201</v>
@@ -6097,7 +6097,7 @@
       <c r="Z83" s="11"/>
       <c r="AA83" s="11"/>
     </row>
-    <row r="84" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L84" s="8"/>
       <c r="M84" s="22" t="s">
         <v>202</v>
@@ -6114,7 +6114,7 @@
       <c r="Z84" s="11"/>
       <c r="AA84" s="11"/>
     </row>
-    <row r="85" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L85" s="8"/>
       <c r="M85" s="9" t="s">
         <v>203</v>
@@ -6131,7 +6131,7 @@
       <c r="Z85" s="11"/>
       <c r="AA85" s="11"/>
     </row>
-    <row r="86" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L86" s="8"/>
       <c r="M86" s="22" t="s">
         <v>204</v>
@@ -6147,7 +6147,7 @@
       <c r="Z86" s="11"/>
       <c r="AA86" s="11"/>
     </row>
-    <row r="87" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L87" s="8"/>
       <c r="M87" s="9" t="s">
         <v>205</v>
@@ -6163,7 +6163,7 @@
       <c r="Z87" s="11"/>
       <c r="AA87" s="11"/>
     </row>
-    <row r="88" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
       <c r="N88" s="15"/>
@@ -6177,7 +6177,7 @@
       <c r="Z88" s="11"/>
       <c r="AA88" s="11"/>
     </row>
-    <row r="89" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L89" s="35" t="s">
         <v>206</v>
       </c>
@@ -6195,7 +6195,7 @@
       <c r="Z89" s="11"/>
       <c r="AA89" s="11"/>
     </row>
-    <row r="90" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L90" s="35" t="s">
         <v>208</v>
       </c>
@@ -6213,7 +6213,7 @@
       <c r="Z90" s="11"/>
       <c r="AA90" s="11"/>
     </row>
-    <row r="91" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L91" s="35" t="s">
         <v>210</v>
       </c>
@@ -6232,7 +6232,7 @@
       <c r="Z91" s="11"/>
       <c r="AA91" s="11"/>
     </row>
-    <row r="92" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R92" s="10"/>
       <c r="U92" s="5"/>
       <c r="W92" s="11"/>
@@ -6241,7 +6241,7 @@
       <c r="Z92" s="11"/>
       <c r="AA92" s="11"/>
     </row>
-    <row r="93" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R93" s="10"/>
       <c r="U93" s="5"/>
       <c r="W93" s="11"/>
@@ -6250,7 +6250,7 @@
       <c r="Z93" s="11"/>
       <c r="AA93" s="11"/>
     </row>
-    <row r="94" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R94" s="10"/>
       <c r="U94" s="5"/>
       <c r="W94" s="11"/>
@@ -6259,7 +6259,7 @@
       <c r="Z94" s="11"/>
       <c r="AA94" s="11"/>
     </row>
-    <row r="95" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R95" s="10"/>
       <c r="U95" s="5"/>
       <c r="W95" s="11"/>
@@ -6268,7 +6268,7 @@
       <c r="Z95" s="11"/>
       <c r="AA95" s="11"/>
     </row>
-    <row r="96" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="12:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R96" s="10"/>
       <c r="U96" s="5"/>
       <c r="W96" s="11"/>
@@ -6277,11 +6277,11 @@
       <c r="Z96" s="11"/>
       <c r="AA96" s="11"/>
     </row>
-    <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="83" t="s">
+    <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="B97" s="72"/>
+      <c r="B97" s="73"/>
       <c r="L97" s="11"/>
       <c r="M97" s="11"/>
       <c r="N97" s="11"/>
@@ -6296,7 +6296,7 @@
       <c r="Z97" s="11"/>
       <c r="AA97" s="11"/>
     </row>
-    <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="40" t="s">
         <v>213</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="Z98" s="11"/>
       <c r="AA98" s="11"/>
     </row>
-    <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>215</v>
       </c>
@@ -6350,7 +6350,7 @@
       <c r="Z99" s="11"/>
       <c r="AA99" s="11"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
@@ -6371,7 +6371,7 @@
       <c r="Z100" s="11"/>
       <c r="AA100" s="11"/>
     </row>
-    <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="22" t="s">
         <v>217</v>
       </c>
@@ -6403,7 +6403,7 @@
       <c r="Z101" s="11"/>
       <c r="AA101" s="11"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>221</v>
       </c>
@@ -6434,7 +6434,7 @@
       <c r="Z102" s="11"/>
       <c r="AA102" s="11"/>
     </row>
-    <row r="103" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="22" t="s">
         <v>225</v>
       </c>
@@ -6466,7 +6466,7 @@
       <c r="Z103" s="11"/>
       <c r="AA103" s="11"/>
     </row>
-    <row r="104" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>229</v>
       </c>
@@ -6498,7 +6498,7 @@
       <c r="Z104" s="11"/>
       <c r="AA104" s="11"/>
     </row>
-    <row r="105" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="22" t="s">
         <v>233</v>
       </c>
@@ -6531,7 +6531,7 @@
       <c r="Z105" s="11"/>
       <c r="AA105" s="11"/>
     </row>
-    <row r="106" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="E106" s="43" t="s">
         <v>237</v>
@@ -6558,7 +6558,7 @@
       <c r="Z106" s="11"/>
       <c r="AA106" s="11"/>
     </row>
-    <row r="107" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
@@ -6579,7 +6579,7 @@
       <c r="Z107" s="11"/>
       <c r="AA107" s="11"/>
     </row>
-    <row r="108" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="40" t="s">
         <v>239</v>
       </c>
@@ -6605,7 +6605,7 @@
       <c r="Z108" s="11"/>
       <c r="AA108" s="11"/>
     </row>
-    <row r="109" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>241</v>
       </c>
@@ -6623,7 +6623,7 @@
       <c r="Z109" s="11"/>
       <c r="AA109" s="11"/>
     </row>
-    <row r="110" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="G110" s="22" t="s">
         <v>242</v>
@@ -6648,7 +6648,7 @@
       <c r="Z110" s="11"/>
       <c r="AA110" s="11"/>
     </row>
-    <row r="111" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="22" t="s">
         <v>244</v>
       </c>
@@ -6681,7 +6681,7 @@
       <c r="Z111" s="11"/>
       <c r="AA111" s="11"/>
     </row>
-    <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>248</v>
       </c>
@@ -6691,7 +6691,7 @@
       <c r="G112" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="H112" s="84" t="s">
+      <c r="H112" s="71" t="s">
         <v>251</v>
       </c>
       <c r="I112" s="68"/>
@@ -6711,7 +6711,7 @@
       <c r="Z112" s="11"/>
       <c r="AA112" s="11"/>
     </row>
-    <row r="113" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="22" t="s">
         <v>252</v>
       </c>
@@ -6742,7 +6742,7 @@
       <c r="Z113" s="11"/>
       <c r="AA113" s="11"/>
     </row>
-    <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>255</v>
       </c>
@@ -6768,7 +6768,7 @@
       <c r="Z114" s="11"/>
       <c r="AA114" s="11"/>
     </row>
-    <row r="115" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="22" t="s">
         <v>257</v>
       </c>
@@ -6799,7 +6799,7 @@
       <c r="Z115" s="11"/>
       <c r="AA115" s="11"/>
     </row>
-    <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>260</v>
       </c>
@@ -6827,7 +6827,7 @@
       <c r="Z116" s="11"/>
       <c r="AA116" s="11"/>
     </row>
-    <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="31"/>
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
@@ -6848,7 +6848,7 @@
       <c r="Z117" s="11"/>
       <c r="AA117" s="11"/>
     </row>
-    <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="22" t="s">
         <v>263</v>
       </c>
@@ -6881,7 +6881,7 @@
       <c r="Z118" s="11"/>
       <c r="AA118" s="11"/>
     </row>
-    <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>267</v>
       </c>
@@ -6911,7 +6911,7 @@
       <c r="Z119" s="11"/>
       <c r="AA119" s="11"/>
     </row>
-    <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4"/>
       <c r="G120" s="22" t="s">
         <v>271</v>
@@ -6936,7 +6936,7 @@
       <c r="Z120" s="11"/>
       <c r="AA120" s="11"/>
     </row>
-    <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="22" t="s">
         <v>273</v>
       </c>
@@ -6965,7 +6965,7 @@
       <c r="Z121" s="11"/>
       <c r="AA121" s="11"/>
     </row>
-    <row r="122" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>275</v>
       </c>
@@ -6991,7 +6991,7 @@
       <c r="Z122" s="11"/>
       <c r="AA122" s="11"/>
     </row>
-    <row r="123" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="G123" s="40" t="s">
         <v>277</v>
@@ -7014,7 +7014,7 @@
       <c r="Z123" s="11"/>
       <c r="AA123" s="11"/>
     </row>
-    <row r="124" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="40" t="s">
         <v>278</v>
       </c>
@@ -7040,7 +7040,7 @@
       <c r="Z124" s="11"/>
       <c r="AA124" s="11"/>
     </row>
-    <row r="125" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
@@ -7061,7 +7061,7 @@
       <c r="Z125" s="11"/>
       <c r="AA125" s="11"/>
     </row>
-    <row r="126" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
         <v>273</v>
       </c>
@@ -7093,7 +7093,7 @@
       <c r="Z126" s="11"/>
       <c r="AA126" s="11"/>
     </row>
-    <row r="127" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>283</v>
       </c>
@@ -7123,7 +7123,7 @@
       <c r="Z127" s="11"/>
       <c r="AA127" s="11"/>
     </row>
-    <row r="128" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
         <v>287</v>
       </c>
@@ -7151,7 +7151,7 @@
       <c r="Z128" s="11"/>
       <c r="AA128" s="11"/>
     </row>
-    <row r="129" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
@@ -7172,7 +7172,7 @@
       <c r="Z129" s="11"/>
       <c r="AA129" s="11"/>
     </row>
-    <row r="130" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
@@ -7193,7 +7193,7 @@
       <c r="Z130" s="11"/>
       <c r="AA130" s="11"/>
     </row>
-    <row r="131" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="40" t="s">
         <v>289</v>
       </c>
@@ -7217,7 +7217,7 @@
       <c r="Z131" s="11"/>
       <c r="AA131" s="11"/>
     </row>
-    <row r="132" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
@@ -7238,7 +7238,7 @@
       <c r="Z132" s="11"/>
       <c r="AA132" s="11"/>
     </row>
-    <row r="133" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="22" t="s">
         <v>290</v>
       </c>
@@ -7267,7 +7267,7 @@
       <c r="Z133" s="11"/>
       <c r="AA133" s="11"/>
     </row>
-    <row r="134" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>292</v>
       </c>
@@ -7293,7 +7293,7 @@
       <c r="Z134" s="11"/>
       <c r="AA134" s="11"/>
     </row>
-    <row r="135" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
         <v>294</v>
       </c>
@@ -7322,7 +7322,7 @@
       <c r="Z135" s="11"/>
       <c r="AA135" s="11"/>
     </row>
-    <row r="136" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>296</v>
       </c>
@@ -7348,7 +7348,7 @@
       <c r="Z136" s="11"/>
       <c r="AA136" s="11"/>
     </row>
-    <row r="137" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
         <v>298</v>
       </c>
@@ -7377,7 +7377,7 @@
       <c r="Z137" s="11"/>
       <c r="AA137" s="11"/>
     </row>
-    <row r="138" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>300</v>
       </c>
@@ -7403,7 +7403,7 @@
       <c r="Z138" s="11"/>
       <c r="AA138" s="11"/>
     </row>
-    <row r="139" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="22" t="s">
         <v>302</v>
       </c>
@@ -7432,7 +7432,7 @@
       <c r="Z139" s="11"/>
       <c r="AA139" s="11"/>
     </row>
-    <row r="140" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
@@ -7453,7 +7453,7 @@
       <c r="Z140" s="11"/>
       <c r="AA140" s="11"/>
     </row>
-    <row r="141" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="G141" s="11"/>
       <c r="H141" s="11"/>
@@ -7474,7 +7474,7 @@
       <c r="Z141" s="11"/>
       <c r="AA141" s="11"/>
     </row>
-    <row r="142" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="G142" s="11"/>
       <c r="H142" s="11"/>
@@ -7495,11 +7495,11 @@
       <c r="Z142" s="11"/>
       <c r="AA142" s="11"/>
     </row>
-    <row r="143" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="85" t="s">
+    <row r="143" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="72" t="s">
         <v>304</v>
       </c>
-      <c r="B143" s="72"/>
+      <c r="B143" s="73"/>
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
       <c r="I143" s="11"/>
@@ -7519,7 +7519,7 @@
       <c r="Z143" s="11"/>
       <c r="AA143" s="11"/>
     </row>
-    <row r="144" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G144" s="11"/>
       <c r="H144" s="11"/>
       <c r="I144" s="11"/>
@@ -7539,8 +7539,8 @@
       <c r="Z144" s="11"/>
       <c r="AA144" s="11"/>
     </row>
-    <row r="145" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="80" t="s">
+    <row r="145" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="74" t="s">
         <v>305</v>
       </c>
       <c r="B145" s="68"/>
@@ -7567,8 +7567,8 @@
       <c r="Z145" s="11"/>
       <c r="AA145" s="11"/>
     </row>
-    <row r="146" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="80" t="s">
+    <row r="146" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="74" t="s">
         <v>309</v>
       </c>
       <c r="B146" s="68"/>
@@ -7592,7 +7592,7 @@
       <c r="Z146" s="11"/>
       <c r="AA146" s="11"/>
     </row>
-    <row r="147" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G147" s="11"/>
       <c r="H147" s="11"/>
       <c r="I147" s="11"/>
@@ -7609,7 +7609,7 @@
       <c r="Z147" s="11"/>
       <c r="AA147" s="11"/>
     </row>
-    <row r="148" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="18" t="s">
         <v>313</v>
       </c>
@@ -7639,7 +7639,7 @@
       <c r="Z148" s="11"/>
       <c r="AA148" s="11"/>
     </row>
-    <row r="149" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>317</v>
       </c>
@@ -7656,7 +7656,7 @@
       </c>
       <c r="Q149" s="11"/>
     </row>
-    <row r="150" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>320</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="151" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>323</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="152" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G152" s="11"/>
       <c r="M152" s="5" t="s">
         <v>326</v>
@@ -7689,29 +7689,29 @@
         <v>327</v>
       </c>
     </row>
-    <row r="153" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>328</v>
       </c>
       <c r="G153" s="11"/>
     </row>
-    <row r="154" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>329</v>
       </c>
       <c r="G154" s="11"/>
     </row>
-    <row r="155" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G155" s="11"/>
     </row>
-    <row r="156" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
         <v>330</v>
       </c>
       <c r="G156" s="11"/>
     </row>
-    <row r="157" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="86" t="s">
+    <row r="157" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="75" t="s">
         <v>331</v>
       </c>
       <c r="B157" s="68"/>
@@ -7721,7 +7721,7 @@
       <c r="F157" s="68"/>
       <c r="G157" s="11"/>
     </row>
-    <row r="158" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="68"/>
       <c r="B158" s="68"/>
       <c r="C158" s="68"/>
@@ -7730,10 +7730,10 @@
       <c r="F158" s="68"/>
       <c r="G158" s="11"/>
     </row>
-    <row r="159" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G159" s="11"/>
     </row>
-    <row r="160" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="27" t="s">
         <v>332</v>
       </c>
@@ -7742,7 +7742,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>334</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G162" s="11"/>
       <c r="M162" s="5" t="s">
         <v>337</v>
@@ -7767,8 +7767,8 @@
         <v>338</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="80" t="s">
+    <row r="163" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="74" t="s">
         <v>339</v>
       </c>
       <c r="B163" s="68"/>
@@ -7780,7 +7780,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>342</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>344</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>346</v>
       </c>
@@ -7810,13 +7810,13 @@
         <v>348</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>349</v>
       </c>
       <c r="G167" s="11"/>
     </row>
-    <row r="168" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G168" s="11"/>
       <c r="L168" s="9" t="s">
         <v>576</v>
@@ -7829,10 +7829,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G169" s="11"/>
     </row>
-    <row r="170" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="11"/>
       <c r="B170" s="11"/>
       <c r="C170" s="11"/>
@@ -7841,7 +7841,7 @@
       <c r="F170" s="11"/>
       <c r="G170" s="11"/>
     </row>
-    <row r="171" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="11"/>
       <c r="B171" s="11"/>
       <c r="C171" s="11"/>
@@ -7850,7 +7850,7 @@
       <c r="F171" s="11"/>
       <c r="G171" s="11"/>
     </row>
-    <row r="172" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="45" t="s">
         <v>352</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>577</v>
       </c>
@@ -7879,7 +7879,7 @@
       </c>
       <c r="M173" s="8"/>
     </row>
-    <row r="174" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="11"/>
       <c r="B174" s="11"/>
       <c r="C174" s="11"/>
@@ -7891,7 +7891,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="22" t="s">
         <v>356</v>
       </c>
@@ -7905,7 +7905,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="10" t="s">
         <v>358</v>
       </c>
@@ -7916,7 +7916,7 @@
       <c r="F176" s="11"/>
       <c r="G176" s="11"/>
     </row>
-    <row r="177" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="10" t="s">
         <v>578</v>
       </c>
@@ -7927,20 +7927,20 @@
       <c r="F177" s="11"/>
       <c r="G177" s="11"/>
     </row>
-    <row r="178" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="10"/>
       <c r="B178" s="11"/>
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
-      <c r="F178" s="81"/>
+      <c r="F178" s="76"/>
       <c r="G178" s="68"/>
       <c r="L178" s="22" t="s">
         <v>359</v>
       </c>
       <c r="M178" s="9"/>
     </row>
-    <row r="179" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="25" t="s">
         <v>360</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="25" t="s">
         <v>579</v>
       </c>
@@ -7969,7 +7969,7 @@
       <c r="F180" s="11"/>
       <c r="G180" s="11"/>
     </row>
-    <row r="181" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>580</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>581</v>
       </c>
@@ -7985,42 +7985,42 @@
         <v>365</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="22" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>373</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>375</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
         <v>377</v>
       </c>
@@ -8044,43 +8044,43 @@
         <v>378</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="22" t="s">
         <v>382</v>
       </c>
       <c r="B208" s="8"/>
     </row>
-    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>584</v>
       </c>
@@ -8088,12 +8088,12 @@
         <v>384</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
         <v>586</v>
       </c>
@@ -8101,7 +8101,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
         <v>386</v>
       </c>
@@ -8109,7 +8109,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
         <v>388</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>390</v>
       </c>
@@ -8125,12 +8125,12 @@
         <v>391</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="48" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="22" t="s">
         <v>393</v>
       </c>
@@ -8139,12 +8139,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="44" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>340</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="22" t="s">
         <v>397</v>
       </c>
@@ -8161,17 +8161,17 @@
         <v>398</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="44" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="22" t="s">
         <v>192</v>
       </c>
@@ -8179,12 +8179,12 @@
         <v>401</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="44" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="22" t="s">
         <v>84</v>
       </c>
@@ -8192,35 +8192,34 @@
         <v>403</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="44" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="19" t="s">
         <v>405</v>
       </c>
       <c r="B251" s="20"/>
     </row>
-    <row r="254" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
         <v>587</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H112:I113"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A157:F158"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="F178:G179"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="G57:J57"/>
     <mergeCell ref="L62:Q62"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:G25"/>
@@ -8229,16 +8228,17 @@
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="K39:L39"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="G57:J57"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="F178:G179"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="H112:I113"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A157:F158"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8253,15 +8253,15 @@
   <dimension ref="A3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="3"/>
+    <col min="1" max="16384" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>406</v>
       </c>
@@ -8269,7 +8269,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>408</v>
       </c>
@@ -8277,7 +8277,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>410</v>
       </c>
@@ -8285,26 +8285,26 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>412</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>414</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>415</v>
       </c>
@@ -8321,22 +8321,22 @@
   </sheetPr>
   <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="3"/>
+    <col min="1" max="16384" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>416</v>
       </c>
       <c r="B1" s="52"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
         <v>417</v>
       </c>
@@ -8346,7 +8346,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>413</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>419</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>421</v>
       </c>
@@ -8378,22 +8378,22 @@
         <v>422</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="53" t="s">
         <v>423</v>
       </c>
       <c r="B7" s="54"/>
       <c r="C7" s="55"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
         <v>425</v>
       </c>
@@ -8405,7 +8405,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>426</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
         <v>428</v>
       </c>
@@ -8434,7 +8434,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>429</v>
       </c>
@@ -8451,7 +8451,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -8464,7 +8464,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>431</v>
       </c>
@@ -8485,7 +8485,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>435</v>
       </c>
@@ -8496,7 +8496,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -8505,7 +8505,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>436</v>
       </c>
@@ -8516,7 +8516,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
         <v>437</v>
@@ -8529,7 +8529,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="4" t="s">
         <v>439</v>
@@ -8542,7 +8542,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
         <v>441</v>
@@ -8555,7 +8555,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -8564,7 +8564,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -8573,7 +8573,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="53" t="s">
         <v>443</v>
       </c>
@@ -8584,7 +8584,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>444</v>
       </c>
@@ -8597,7 +8597,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -8606,7 +8606,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>446</v>
       </c>
@@ -8619,7 +8619,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>448</v>
       </c>
@@ -8632,7 +8632,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="56" t="s">
         <v>450</v>
       </c>
@@ -8650,7 +8650,7 @@
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="53" t="s">
         <v>451</v>
       </c>
@@ -8668,7 +8668,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>452</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>454</v>
       </c>
@@ -8708,7 +8708,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -8724,7 +8724,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>456</v>
       </c>
@@ -8744,7 +8744,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="4" t="s">
         <v>458</v>
@@ -8762,7 +8762,7 @@
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="4" t="s">
         <v>459</v>
@@ -8780,7 +8780,7 @@
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="4" t="s">
         <v>460</v>
@@ -8798,7 +8798,7 @@
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="4" t="s">
         <v>461</v>
@@ -8816,7 +8816,7 @@
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
     </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="4" t="s">
         <v>462</v>
@@ -8834,7 +8834,7 @@
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
     </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="49" t="s">
@@ -8852,7 +8852,7 @@
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -8868,7 +8868,7 @@
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>464</v>
       </c>
@@ -8888,7 +8888,7 @@
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>466</v>
       </c>
@@ -8910,7 +8910,7 @@
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -8926,7 +8926,7 @@
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>469</v>
       </c>
@@ -8948,7 +8948,7 @@
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>472</v>
       </c>
@@ -8968,7 +8968,7 @@
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -8986,7 +8986,7 @@
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -9004,7 +9004,7 @@
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
     </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -9022,7 +9022,7 @@
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
     </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -9040,7 +9040,7 @@
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -9057,7 +9057,7 @@
       <c r="M59" s="5"/>
       <c r="N59" s="5"/>
     </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>479</v>
       </c>
@@ -9077,7 +9077,7 @@
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
     </row>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>481</v>
       </c>
@@ -9097,7 +9097,7 @@
       <c r="M61" s="5"/>
       <c r="N61" s="5"/>
     </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -9113,7 +9113,7 @@
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
     </row>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>483</v>
       </c>
@@ -9133,7 +9133,7 @@
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -9149,7 +9149,7 @@
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
     </row>
-    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>485</v>
       </c>
@@ -9169,7 +9169,7 @@
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
     </row>
-    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>588</v>
       </c>
@@ -9187,7 +9187,7 @@
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
     </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -9203,7 +9203,7 @@
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
     </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>487</v>
       </c>
@@ -9223,7 +9223,7 @@
       <c r="M68" s="5"/>
       <c r="N68" s="5"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -9239,7 +9239,7 @@
       <c r="M69" s="5"/>
       <c r="N69" s="5"/>
     </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -9255,7 +9255,7 @@
       <c r="M70" s="5"/>
       <c r="N70" s="5"/>
     </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -9271,7 +9271,7 @@
       <c r="M71" s="5"/>
       <c r="N71" s="5"/>
     </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="53" t="s">
         <v>489</v>
       </c>
@@ -9289,7 +9289,7 @@
       <c r="M72" s="5"/>
       <c r="N72" s="5"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>490</v>
       </c>
@@ -9309,7 +9309,7 @@
       <c r="M73" s="5"/>
       <c r="N73" s="5"/>
     </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -9325,7 +9325,7 @@
       <c r="M74" s="5"/>
       <c r="N74" s="5"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>456</v>
       </c>
@@ -9345,7 +9345,7 @@
       <c r="M75" s="5"/>
       <c r="N75" s="5"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="4" t="s">
         <v>493</v>
@@ -9363,7 +9363,7 @@
       <c r="M76" s="5"/>
       <c r="N76" s="5"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="49" t="s">
@@ -9381,7 +9381,7 @@
       <c r="M77" s="5"/>
       <c r="N77" s="5"/>
     </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -9397,7 +9397,7 @@
       <c r="M78" s="5"/>
       <c r="N78" s="5"/>
     </row>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
@@ -9413,7 +9413,7 @@
       <c r="M79" s="5"/>
       <c r="N79" s="5"/>
     </row>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>494</v>
       </c>
@@ -9433,7 +9433,7 @@
       <c r="M80" s="5"/>
       <c r="N80" s="5"/>
     </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
@@ -9449,7 +9449,7 @@
       <c r="M81" s="5"/>
       <c r="N81" s="5"/>
     </row>
-    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>496</v>
       </c>
@@ -9469,7 +9469,7 @@
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
     </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>498</v>
       </c>
@@ -9487,13 +9487,13 @@
       <c r="M83" s="5"/>
       <c r="N83" s="5"/>
     </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="56" t="s">
         <v>499</v>
       </c>
       <c r="B92" s="57"/>
     </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>500</v>
       </c>
@@ -9508,7 +9508,7 @@
       </c>
       <c r="I94" s="5"/>
     </row>
-    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -9519,7 +9519,7 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
     </row>
-    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
@@ -9530,7 +9530,7 @@
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
     </row>
-    <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="58" t="s">
         <v>502</v>
       </c>
@@ -9543,7 +9543,7 @@
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
     </row>
-    <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>503</v>
       </c>
@@ -9558,7 +9558,7 @@
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
     </row>
-    <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>505</v>
       </c>
@@ -9571,7 +9571,7 @@
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
     </row>
-    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -9582,7 +9582,7 @@
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
     </row>
-    <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>506</v>
       </c>
@@ -9595,7 +9595,7 @@
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
     </row>
-    <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>507</v>
       </c>
@@ -9608,7 +9608,7 @@
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
     </row>
-    <row r="105" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="56" t="s">
         <v>508</v>
       </c>
@@ -9617,12 +9617,12 @@
       <c r="D105" s="57"/>
       <c r="E105" s="57"/>
     </row>
-    <row r="106" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>510</v>
       </c>
@@ -9646,12 +9646,12 @@
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="3"/>
+    <col min="1" max="16384" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="88"/>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
@@ -9666,7 +9666,7 @@
       <c r="L1" s="68"/>
       <c r="M1" s="68"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
@@ -9681,7 +9681,7 @@
       <c r="L2" s="68"/>
       <c r="M2" s="68"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="68"/>
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
@@ -9696,17 +9696,17 @@
       <c r="L3" s="68"/>
       <c r="M3" s="68"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>513</v>
       </c>
@@ -9718,7 +9718,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>516</v>
       </c>
@@ -9734,7 +9734,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>519</v>
       </c>
@@ -9745,39 +9745,39 @@
         <v>521</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="9" t="s">
         <v>522</v>
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>524</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>592</v>
       </c>
@@ -9788,12 +9788,12 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>594</v>
       </c>
@@ -9810,7 +9810,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="60" t="s">
         <v>525</v>
       </c>
@@ -9824,7 +9824,7 @@
       </c>
       <c r="F27" s="62"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="63" t="s">
         <v>528</v>
       </c>
@@ -9837,7 +9837,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="63" t="s">
         <v>531</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="63" t="s">
         <v>534</v>
       </c>
@@ -9863,7 +9863,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="63" t="s">
         <v>537</v>
       </c>
@@ -9876,7 +9876,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="63" t="s">
         <v>540</v>
       </c>
@@ -9889,7 +9889,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="63" t="s">
         <v>543</v>
       </c>

</xml_diff>